<commit_message>
fix bug with grouping sourcing
</commit_message>
<xml_diff>
--- a/Action items tracking.xlsx
+++ b/Action items tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangken/py/pcba_allocation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F716553-F2A0-8D4E-9532-86D7E907E308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FAE654-7D18-9048-873F-5E5F906A8273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" xr2:uid="{0EAF019F-23F5-0949-BFD7-20AFE2D07F98}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Item</t>
   </si>
@@ -108,21 +108,23 @@
     <t>Action summary</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Mandy working with Amit for long term solution;
+    <t xml:space="preserve"> - To be further discussed/aligned</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - To be further discussed/aligned for EDI allocation need and logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Longer term solution: Mandy working with Amit;
  - Short term solution: Use smartsheet as workaround to put in the missing intransit data</t>
   </si>
   <si>
-    <t>Ken working with InfoSec team for access. ETA: Dec 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - To be discussed if different logic needed;
- - Propose to add in to consider YE orders following Current FCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - To be further discussed/aligned</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - To be further discussed/aligned for EDI allocation need and logic</t>
+    <t>Ken working with InfoSec team to fix firewall issue. ETA: Dec 25</t>
+  </si>
+  <si>
+    <t>On-going discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Continue to align with PSP/DF Mgr/Central to adjust logic as needed</t>
   </si>
 </sst>
 </file>
@@ -145,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +178,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -239,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -272,14 +280,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,7 +609,7 @@
   <dimension ref="B5:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="112" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +618,7 @@
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
     <col min="3" max="3" width="48.6640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="59.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" style="4" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" customWidth="1"/>
   </cols>
@@ -622,14 +633,14 @@
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="9" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="B6" s="6">
         <v>1</v>
       </c>
@@ -639,11 +650,11 @@
       <c r="D6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:6" s="9" customFormat="1" ht="68" x14ac:dyDescent="0.2">
@@ -656,14 +667,14 @@
       <c r="D7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" s="9" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <v>3</v>
       </c>
@@ -673,11 +684,11 @@
       <c r="D8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>9</v>
+      <c r="E8" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:6" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -690,11 +701,11 @@
       <c r="D9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:6" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -707,11 +718,11 @@
       <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:6" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">

</xml_diff>